<commit_message>
al kindi al farabi ibn sina
</commit_message>
<xml_diff>
--- a/DigSite/New Arcaism/uarm 2024 2/omfg pls no nooo.xlsx
+++ b/DigSite/New Arcaism/uarm 2024 2/omfg pls no nooo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitData\ArchaeologyJourney\DigSite\New Arcaism\uarm 2024 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FDD76C2-F50D-4C24-A063-23E6339D5D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F54E24-F483-4C07-83F9-7339BE916F6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9165" yWindow="195" windowWidth="10845" windowHeight="10725" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="2430" windowWidth="10845" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:F4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,21 +503,33 @@
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C6">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C8">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C9">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -533,73 +545,94 @@
       <c r="B12" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>27</v>
       </c>

</xml_diff>